<commit_message>
Updated research data to reflect re-assessment of a detection tool performance
</commit_message>
<xml_diff>
--- a/researchData/TOPSISAnalysis/DetectionPerformance_TOPSIS.xlsx
+++ b/researchData/TOPSISAnalysis/DetectionPerformance_TOPSIS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Backups\Mestrado\Prepd_Ano2_Semestre1\Dissertacao\Documentos Meus Apoio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC5FBBC-F79C-4377-AF9F-F6F2DC7B9273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82F09B7-7237-411F-B6AB-044F317A99EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{31F6B3F9-68F3-43F3-B007-3B3089A69F57}"/>
   </bookViews>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6152535D-20AE-4B6B-93B2-B6459BC5390F}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,13 +602,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="C5" s="2">
         <v>0.56999999999999995</v>
       </c>
       <c r="D5" s="2">
-        <v>3146</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -738,13 +738,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="2">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="C29" s="2">
         <v>0.56999999999999995</v>
       </c>
       <c r="D29" s="2">
-        <v>3146</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -801,16 +801,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="2">
-        <f>POWER(B29,2)</f>
-        <v>0.60840000000000005</v>
+        <f t="shared" ref="B37:D39" si="0">POWER(B29,2)</f>
+        <v>0.59289999999999998</v>
       </c>
       <c r="C37" s="2">
-        <f>POWER(C29,2)</f>
+        <f t="shared" si="0"/>
         <v>0.32489999999999997</v>
       </c>
       <c r="D37" s="2">
-        <f>POWER(D29,2)</f>
-        <v>9897316</v>
+        <f t="shared" si="0"/>
+        <v>6225025</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,15 +818,15 @@
         <v>1</v>
       </c>
       <c r="B38" s="2">
-        <f>POWER(B30,2)</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000005E-3</v>
       </c>
       <c r="C38" s="2">
-        <f>POWER(C30,2)</f>
+        <f t="shared" si="0"/>
         <v>4.8399999999999999E-2</v>
       </c>
       <c r="D38" s="2">
-        <f>POWER(D30,2)</f>
+        <f t="shared" si="0"/>
         <v>2114116</v>
       </c>
     </row>
@@ -835,15 +835,15 @@
         <v>3</v>
       </c>
       <c r="B39" s="2">
-        <f>POWER(B31,2)</f>
+        <f t="shared" si="0"/>
         <v>1E-4</v>
       </c>
       <c r="C39" s="2">
-        <f>POWER(C31,2)</f>
+        <f t="shared" si="0"/>
         <v>1.6900000000000002E-2</v>
       </c>
       <c r="D39" s="2">
-        <f>POWER(D31,2)</f>
+        <f t="shared" si="0"/>
         <v>3308761</v>
       </c>
     </row>
@@ -853,15 +853,15 @@
       </c>
       <c r="B40" s="7">
         <f>SUM(B37:B39)</f>
-        <v>0.61099999999999999</v>
+        <v>0.59549999999999992</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" ref="C40:D40" si="0">SUM(C37:C39)</f>
+        <f t="shared" ref="C40:D40" si="1">SUM(C37:C39)</f>
         <v>0.39019999999999999</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="0"/>
-        <v>15320193</v>
+        <f t="shared" si="1"/>
+        <v>11647902</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -870,15 +870,15 @@
       </c>
       <c r="B41" s="7">
         <f>SQRT(B40)</f>
-        <v>0.7816648898345121</v>
+        <v>0.77168646482881886</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" ref="C41:D41" si="1">SQRT(C40)</f>
+        <f t="shared" ref="C41:D41" si="2">SQRT(C40)</f>
         <v>0.62465990746965661</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="1"/>
-        <v>3914.101812676824</v>
+        <f t="shared" si="2"/>
+        <v>3412.9022839806007</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,7 +903,7 @@
       </c>
       <c r="B46" s="2">
         <f>B29/$B$41</f>
-        <v>0.99787007212916456</v>
+        <v>0.99781457249066441</v>
       </c>
       <c r="C46" s="2">
         <f>C29/$C$41</f>
@@ -911,7 +911,7 @@
       </c>
       <c r="D46" s="2">
         <f>1 - D29/$D$41</f>
-        <v>0.19623960986122768</v>
+        <v>0.26895064892101617</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
       </c>
       <c r="B47" s="2">
         <f>B30/$B$41</f>
-        <v>6.3966030264690041E-2</v>
+        <v>6.4793154057835353E-2</v>
       </c>
       <c r="C47" s="2">
         <f>C30/$C$41</f>
@@ -928,7 +928,7 @@
       </c>
       <c r="D47" s="2">
         <f>1 - D30/$D$41</f>
-        <v>0.62852269317807541</v>
+        <v>0.57396963668583467</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -937,7 +937,7 @@
       </c>
       <c r="B48" s="2">
         <f>B31/$B$41</f>
-        <v>1.2793206052938006E-2</v>
+        <v>1.2958630811567069E-2</v>
       </c>
       <c r="C48" s="2">
         <f>C31/$C$41</f>
@@ -945,7 +945,7 @@
       </c>
       <c r="D48" s="2">
         <f>1 - D31/$D$41</f>
-        <v>0.53527013678880264</v>
+        <v>0.46702253722939013</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
       </c>
       <c r="B54" s="2">
         <f>B46*$B$27</f>
-        <v>0.49893503606458228</v>
+        <v>0.4989072862453322</v>
       </c>
       <c r="C54" s="2">
         <f>C46*$C$27</f>
@@ -978,7 +978,7 @@
       </c>
       <c r="D54" s="2">
         <f>D46*$D$27</f>
-        <v>5.8871882958368302E-2</v>
+        <v>8.0685194676304847E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -987,7 +987,7 @@
       </c>
       <c r="B55" s="2">
         <f>B47*$B$27</f>
-        <v>3.198301513234502E-2</v>
+        <v>3.2396577028917677E-2</v>
       </c>
       <c r="C55" s="2">
         <f>C47*$C$27</f>
@@ -995,7 +995,7 @@
       </c>
       <c r="D55" s="2">
         <f>D47*$D$27</f>
-        <v>0.18855680795342261</v>
+        <v>0.17219089100575038</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B56" s="2">
         <f>B48*$B$27</f>
-        <v>6.396603026469003E-3</v>
+        <v>6.4793154057835346E-3</v>
       </c>
       <c r="C56" s="2">
         <f>C48*$C$27</f>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="D56" s="2">
         <f>D48*$D$27</f>
-        <v>0.16058104103664078</v>
+        <v>0.14010676116881704</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1037,15 +1037,15 @@
       </c>
       <c r="B66" s="2">
         <f>B54</f>
-        <v>0.49893503606458228</v>
+        <v>0.4989072862453322</v>
       </c>
       <c r="C66" s="2">
-        <f t="shared" ref="C66:D66" si="2">C54</f>
+        <f t="shared" ref="C66:D66" si="3">C54</f>
         <v>0.18249930664157063</v>
       </c>
       <c r="D66" s="2">
-        <f t="shared" si="2"/>
-        <v>5.8871882958368302E-2</v>
+        <f t="shared" si="3"/>
+        <v>8.0685194676304847E-2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1053,16 +1053,16 @@
         <v>1</v>
       </c>
       <c r="B67" s="2">
-        <f t="shared" ref="B67:D68" si="3">B55</f>
-        <v>3.198301513234502E-2</v>
+        <f t="shared" ref="B67:D68" si="4">B55</f>
+        <v>3.2396577028917677E-2</v>
       </c>
       <c r="C67" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.0438328879202705E-2</v>
       </c>
       <c r="D67" s="2">
-        <f t="shared" si="3"/>
-        <v>0.18855680795342261</v>
+        <f t="shared" si="4"/>
+        <v>0.17219089100575038</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1070,16 +1070,16 @@
         <v>3</v>
       </c>
       <c r="B68" s="2">
-        <f t="shared" si="3"/>
-        <v>6.396603026469003E-3</v>
+        <f t="shared" si="4"/>
+        <v>6.4793154057835346E-3</v>
       </c>
       <c r="C68" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1622648883165241E-2</v>
       </c>
       <c r="D68" s="2">
-        <f t="shared" si="3"/>
-        <v>0.16058104103664078</v>
+        <f t="shared" si="4"/>
+        <v>0.14010676116881704</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B69" s="7">
         <f>MAX(B66:B68)</f>
-        <v>0.49893503606458228</v>
+        <v>0.4989072862453322</v>
       </c>
       <c r="C69" s="7">
         <f>MAX(C66:C68)</f>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="D69" s="7">
         <f>MAX(D66:D68)</f>
-        <v>0.18855680795342261</v>
+        <v>0.17219089100575038</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1120,16 +1120,16 @@
         <v>2</v>
       </c>
       <c r="B78" s="2">
-        <f>B54</f>
-        <v>0.49893503606458228</v>
+        <f t="shared" ref="B78:D80" si="5">B54</f>
+        <v>0.4989072862453322</v>
       </c>
       <c r="C78" s="2">
-        <f>C54</f>
+        <f t="shared" si="5"/>
         <v>0.18249930664157063</v>
       </c>
       <c r="D78" s="2">
-        <f>D54</f>
-        <v>5.8871882958368302E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.0685194676304847E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1137,16 +1137,16 @@
         <v>1</v>
       </c>
       <c r="B79" s="2">
-        <f>B55</f>
-        <v>3.198301513234502E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.2396577028917677E-2</v>
       </c>
       <c r="C79" s="2">
-        <f>C55</f>
+        <f t="shared" si="5"/>
         <v>7.0438328879202705E-2</v>
       </c>
       <c r="D79" s="2">
-        <f>D55</f>
-        <v>0.18855680795342261</v>
+        <f t="shared" si="5"/>
+        <v>0.17219089100575038</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1154,16 +1154,16 @@
         <v>3</v>
       </c>
       <c r="B80" s="2">
-        <f>B56</f>
-        <v>6.396603026469003E-3</v>
+        <f t="shared" si="5"/>
+        <v>6.4793154057835346E-3</v>
       </c>
       <c r="C80" s="2">
-        <f>C56</f>
+        <f t="shared" si="5"/>
         <v>4.1622648883165241E-2</v>
       </c>
       <c r="D80" s="2">
-        <f>D56</f>
-        <v>0.16058104103664078</v>
+        <f t="shared" si="5"/>
+        <v>0.14010676116881704</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B81" s="7">
         <f>MIN(B78:B80)</f>
-        <v>6.396603026469003E-3</v>
+        <v>6.4793154057835346E-3</v>
       </c>
       <c r="C81" s="7">
         <f>MIN(C78:C80)</f>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="D81" s="7">
         <f>MIN(D78:D80)</f>
-        <v>5.8871882958368302E-2</v>
+        <v>8.0685194676304847E-2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D90" s="2">
         <f>(D54-$D$69)^2</f>
-        <v>1.6818179770972858E-2</v>
+        <v>8.3732924607367032E-3</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B91" s="2">
         <f>(B55-$B$69)^2</f>
-        <v>0.21804418985270055</v>
+        <v>0.21763224181360205</v>
       </c>
       <c r="C91" s="2">
         <f>(C55-$C$69)^2</f>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B92" s="2">
         <f>(B56-$B$69)^2</f>
-        <v>0.24259410801964001</v>
+        <v>0.24248530646515537</v>
       </c>
       <c r="C92" s="2">
         <f>(C56-$C$69)^2</f>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="D92" s="2">
         <f>(D56-$D$69)^2</f>
-        <v>7.8264353458210479E-4</v>
+        <v>1.0293913873931965E-3</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,12 +1273,12 @@
         <v>2</v>
       </c>
       <c r="B97" s="2">
-        <f t="shared" ref="B97:B98" si="4">SUM(B90:D90)</f>
-        <v>1.6818179770972858E-2</v>
+        <f t="shared" ref="B97:B98" si="6">SUM(B90:D90)</f>
+        <v>8.3732924607367032E-3</v>
       </c>
       <c r="C97" s="2">
         <f>SQRT(B97)</f>
-        <v>0.1296849249950543</v>
+        <v>9.1505696329445538E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -1286,12 +1286,12 @@
         <v>1</v>
       </c>
       <c r="B98" s="2">
-        <f t="shared" si="4"/>
-        <v>0.23060185258975846</v>
+        <f t="shared" si="6"/>
+        <v>0.23018990455065996</v>
       </c>
       <c r="C98" s="2">
-        <f t="shared" ref="C98:C99" si="5">SQRT(B98)</f>
-        <v>0.48021021708180933</v>
+        <f t="shared" ref="C98:C99" si="7">SQRT(B98)</f>
+        <v>0.47978110066014479</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -1300,11 +1300,11 @@
       </c>
       <c r="B99" s="2">
         <f>SUM(B92:D92)</f>
-        <v>0.26322298425540103</v>
+        <v>0.26336093055372745</v>
       </c>
       <c r="C99" s="2">
-        <f t="shared" si="5"/>
-        <v>0.51305261353529918</v>
+        <f t="shared" si="7"/>
+        <v>0.51318703272172361</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B107" s="2">
         <f>(B54-$B$81)^2</f>
-        <v>0.24259410801964001</v>
+        <v>0.24248530646515537</v>
       </c>
       <c r="C107" s="2">
         <f>(C54-$C$81)^2</f>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B108" s="2">
         <f>(B55-$B$81)^2</f>
-        <v>6.5466448445171887E-4</v>
+        <v>6.7170445004198173E-4</v>
       </c>
       <c r="C108" s="2">
         <f>(C55-$C$81)^2</f>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="D108" s="2">
         <f>(D55-$D$81)^2</f>
-        <v>1.6818179770972858E-2</v>
+        <v>8.3732924607367032E-3</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D109" s="2">
         <f>(D56-$D$81)^2</f>
-        <v>1.034475283699102E-2</v>
+        <v>3.5309225644240476E-3</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -1398,11 +1398,11 @@
       </c>
       <c r="B114" s="2">
         <f>SUM(B107:D107)</f>
-        <v>0.2624403407208189</v>
+        <v>0.26233153916633423</v>
       </c>
       <c r="C114" s="2">
         <f>SQRT(B114)</f>
-        <v>0.51228931349464912</v>
+        <v>0.51218311097334535</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -1410,12 +1410,12 @@
         <v>1</v>
       </c>
       <c r="B115" s="2">
-        <f t="shared" ref="B115:B116" si="6">SUM(B108:D108)</f>
-        <v>1.8303187669058609E-2</v>
+        <f t="shared" ref="B115:B116" si="8">SUM(B108:D108)</f>
+        <v>9.8753403244127187E-3</v>
       </c>
       <c r="C115" s="2">
-        <f t="shared" ref="C115:C116" si="7">SQRT(B115)</f>
-        <v>0.13528927403552216</v>
+        <f t="shared" ref="C115:C116" si="9">SQRT(B115)</f>
+        <v>9.9374746914961842E-2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -1423,12 +1423,12 @@
         <v>3</v>
       </c>
       <c r="B116" s="2">
-        <f t="shared" si="6"/>
-        <v>1.034475283699102E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.5309225644240476E-3</v>
       </c>
       <c r="C116" s="2">
-        <f t="shared" si="7"/>
-        <v>0.10170915807827248</v>
+        <f t="shared" si="9"/>
+        <v>5.9421566492512193E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="B122" s="2">
         <f>C114/(C97+C114)</f>
-        <v>0.79799045316810757</v>
+        <v>0.848422407004228</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B123" s="2">
         <f>C115/(C98+C115)</f>
-        <v>0.21980403881395286</v>
+        <v>0.17158550212527143</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B124" s="2">
         <f>C116/(C99+C116)</f>
-        <v>0.16544483208725777</v>
+        <v>0.1037734441537442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>